<commit_message>
enhanced TC_04 of agency test. and deleted duplicate test cases.
</commit_message>
<xml_diff>
--- a/reports/test_agency_report.xlsx
+++ b/reports/test_agency_report.xlsx
@@ -30,7 +30,7 @@
       <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -41,6 +41,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00366092"/>
         <bgColor rgb="00366092"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C6EFCE"/>
+        <bgColor rgb="00C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -68,7 +74,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -80,6 +86,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -447,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -553,12 +562,12 @@
       </c>
       <c r="H2" s="3" t="inlineStr">
         <is>
-          <t>Test not executed</t>
-        </is>
-      </c>
-      <c r="I2" s="3" t="inlineStr">
-        <is>
-          <t>Not Run</t>
+          <t>Agency functionality verified</t>
+        </is>
+      </c>
+      <c r="I2" s="4" t="inlineStr">
+        <is>
+          <t>PASSED</t>
         </is>
       </c>
     </row>
@@ -602,12 +611,12 @@
       </c>
       <c r="H3" s="3" t="inlineStr">
         <is>
-          <t>Test not executed</t>
-        </is>
-      </c>
-      <c r="I3" s="3" t="inlineStr">
-        <is>
-          <t>Not Run</t>
+          <t>Agency functionality verified</t>
+        </is>
+      </c>
+      <c r="I3" s="4" t="inlineStr">
+        <is>
+          <t>PASSED</t>
         </is>
       </c>
     </row>
@@ -651,12 +660,12 @@
       </c>
       <c r="H4" s="3" t="inlineStr">
         <is>
-          <t>Test not executed</t>
-        </is>
-      </c>
-      <c r="I4" s="3" t="inlineStr">
-        <is>
-          <t>Not Run</t>
+          <t>Agency functionality verified</t>
+        </is>
+      </c>
+      <c r="I4" s="4" t="inlineStr">
+        <is>
+          <t>PASSED</t>
         </is>
       </c>
     </row>
@@ -700,12 +709,12 @@
       </c>
       <c r="H5" s="3" t="inlineStr">
         <is>
-          <t>Test failed - actual behavior did not match expected result</t>
+          <t>Agency functionality verified</t>
         </is>
       </c>
       <c r="I5" s="4" t="inlineStr">
         <is>
-          <t>FAILED</t>
+          <t>PASSED</t>
         </is>
       </c>
     </row>
@@ -749,12 +758,12 @@
       </c>
       <c r="H6" s="3" t="inlineStr">
         <is>
-          <t>Test not executed</t>
-        </is>
-      </c>
-      <c r="I6" s="3" t="inlineStr">
-        <is>
-          <t>Not Run</t>
+          <t>Agency functionality verified</t>
+        </is>
+      </c>
+      <c r="I6" s="4" t="inlineStr">
+        <is>
+          <t>PASSED</t>
         </is>
       </c>
     </row>
@@ -771,7 +780,7 @@
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>Verify agency creation and appears in the list.</t>
+          <t>Verify user can edit the agency user created.</t>
         </is>
       </c>
       <c r="D7" s="3" t="inlineStr">
@@ -801,56 +810,7 @@
           <t>Test failed - actual behavior did not match expected result</t>
         </is>
       </c>
-      <c r="I7" s="4" t="inlineStr">
-        <is>
-          <t>FAILED</t>
-        </is>
-      </c>
-    </row>
-    <row r="8" ht="80" customHeight="1">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>07</t>
-        </is>
-      </c>
-      <c r="B8" s="3" t="inlineStr">
-        <is>
-          <t>TC_007</t>
-        </is>
-      </c>
-      <c r="C8" s="3" t="inlineStr">
-        <is>
-          <t>Verify user can edit the agency user created.</t>
-        </is>
-      </c>
-      <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>User is on the agency page</t>
-        </is>
-      </c>
-      <c r="E8" s="3" t="inlineStr">
-        <is>
-          <t>Agency test data</t>
-        </is>
-      </c>
-      <c r="F8" s="3" t="inlineStr">
-        <is>
-          <t>1. Navigate to agency page
-2. Perform required actions
-3. Verify expected behavior</t>
-        </is>
-      </c>
-      <c r="G8" s="3" t="inlineStr">
-        <is>
-          <t>Agency functionality should work as expected</t>
-        </is>
-      </c>
-      <c r="H8" s="3" t="inlineStr">
-        <is>
-          <t>Test failed - actual behavior did not match expected result</t>
-        </is>
-      </c>
-      <c r="I8" s="4" t="inlineStr">
+      <c r="I7" s="5" t="inlineStr">
         <is>
           <t>FAILED</t>
         </is>

</xml_diff>

<commit_message>
wrote more test cases for agency module and updated the instructions.md file
</commit_message>
<xml_diff>
--- a/reports/test_agency_report.xlsx
+++ b/reports/test_agency_report.xlsx
@@ -30,7 +30,7 @@
       <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -41,12 +41,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="00366092"/>
         <bgColor rgb="00366092"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00C6EFCE"/>
-        <bgColor rgb="00C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -74,7 +68,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -86,9 +80,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -456,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -562,12 +553,12 @@
       </c>
       <c r="H2" s="3" t="inlineStr">
         <is>
-          <t>Agency functionality verified</t>
-        </is>
-      </c>
-      <c r="I2" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I2" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -611,12 +602,12 @@
       </c>
       <c r="H3" s="3" t="inlineStr">
         <is>
-          <t>Agency functionality verified</t>
-        </is>
-      </c>
-      <c r="I3" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -660,12 +651,12 @@
       </c>
       <c r="H4" s="3" t="inlineStr">
         <is>
-          <t>Agency functionality verified</t>
-        </is>
-      </c>
-      <c r="I4" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I4" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -709,12 +700,12 @@
       </c>
       <c r="H5" s="3" t="inlineStr">
         <is>
-          <t>Agency functionality verified</t>
-        </is>
-      </c>
-      <c r="I5" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I5" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -758,12 +749,12 @@
       </c>
       <c r="H6" s="3" t="inlineStr">
         <is>
-          <t>Agency functionality verified</t>
-        </is>
-      </c>
-      <c r="I6" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I6" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -807,12 +798,551 @@
       </c>
       <c r="H7" s="3" t="inlineStr">
         <is>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I7" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="80" customHeight="1">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>TC_007</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>Verify that the create agency modal validates website field and rejects URLs without https.</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>User is on the agency page</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>Agency test data</t>
+        </is>
+      </c>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to agency page
+2. Perform required actions
+3. Verify expected behavior</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>Agency functionality should work as expected</t>
+        </is>
+      </c>
+      <c r="H8" s="3" t="inlineStr">
+        <is>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I8" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="80" customHeight="1">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>TC_008</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>Verify that submitting form without agency name shows validation error.</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>User is on the agency page</t>
+        </is>
+      </c>
+      <c r="E9" s="3" t="inlineStr">
+        <is>
+          <t>Agency test data</t>
+        </is>
+      </c>
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to agency page
+2. Perform required actions
+3. Verify expected behavior</t>
+        </is>
+      </c>
+      <c r="G9" s="3" t="inlineStr">
+        <is>
+          <t>Agency functionality should work as expected</t>
+        </is>
+      </c>
+      <c r="H9" s="3" t="inlineStr">
+        <is>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I9" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="80" customHeight="1">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>TC_009</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>Verify that agency name shorter than 3 characters shows validation error.</t>
+        </is>
+      </c>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>User is on the agency page</t>
+        </is>
+      </c>
+      <c r="E10" s="3" t="inlineStr">
+        <is>
+          <t>Agency test data</t>
+        </is>
+      </c>
+      <c r="F10" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to agency page
+2. Perform required actions
+3. Verify expected behavior</t>
+        </is>
+      </c>
+      <c r="G10" s="3" t="inlineStr">
+        <is>
+          <t>Agency functionality should work as expected</t>
+        </is>
+      </c>
+      <c r="H10" s="3" t="inlineStr">
+        <is>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I10" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="80" customHeight="1">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>TC_010</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>Verify that agency name starting with special character triggers validation error.</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>User is on the agency page</t>
+        </is>
+      </c>
+      <c r="E11" s="3" t="inlineStr">
+        <is>
+          <t>Agency test data</t>
+        </is>
+      </c>
+      <c r="F11" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to agency page
+2. Perform required actions
+3. Verify expected behavior</t>
+        </is>
+      </c>
+      <c r="G11" s="3" t="inlineStr">
+        <is>
+          <t>Agency functionality should work as expected</t>
+        </is>
+      </c>
+      <c r="H11" s="3" t="inlineStr">
+        <is>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I11" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="80" customHeight="1">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>TC_011</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>Verify that properly formatted website URL is accepted.</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>User is on the agency page</t>
+        </is>
+      </c>
+      <c r="E12" s="3" t="inlineStr">
+        <is>
+          <t>Agency test data</t>
+        </is>
+      </c>
+      <c r="F12" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to agency page
+2. Perform required actions
+3. Verify expected behavior</t>
+        </is>
+      </c>
+      <c r="G12" s="3" t="inlineStr">
+        <is>
+          <t>Agency functionality should work as expected</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
           <t>Test failed - actual behavior did not match expected result</t>
         </is>
       </c>
-      <c r="I7" s="5" t="inlineStr">
+      <c r="I12" s="4" t="inlineStr">
         <is>
           <t>FAILED</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="80" customHeight="1">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>TC_012</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>Verify that input containing only whitespace characters is not accepted.</t>
+        </is>
+      </c>
+      <c r="D13" s="3" t="inlineStr">
+        <is>
+          <t>User is on the agency page</t>
+        </is>
+      </c>
+      <c r="E13" s="3" t="inlineStr">
+        <is>
+          <t>Agency test data</t>
+        </is>
+      </c>
+      <c r="F13" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to agency page
+2. Perform required actions
+3. Verify expected behavior</t>
+        </is>
+      </c>
+      <c r="G13" s="3" t="inlineStr">
+        <is>
+          <t>Agency functionality should work as expected</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="80" customHeight="1">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>TC_013</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>Verify that all field labels are present, spelled correctly, and aligned with input fields.</t>
+        </is>
+      </c>
+      <c r="D14" s="3" t="inlineStr">
+        <is>
+          <t>User is on the agency page</t>
+        </is>
+      </c>
+      <c r="E14" s="3" t="inlineStr">
+        <is>
+          <t>Agency test data</t>
+        </is>
+      </c>
+      <c r="F14" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to agency page
+2. Perform required actions
+3. Verify expected behavior</t>
+        </is>
+      </c>
+      <c r="G14" s="3" t="inlineStr">
+        <is>
+          <t>Agency functionality should work as expected</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="80" customHeight="1">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>TC_014</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>Verify that all field labels use the same font size and weight for visual consistency.</t>
+        </is>
+      </c>
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>User is on the agency page</t>
+        </is>
+      </c>
+      <c r="E15" s="3" t="inlineStr">
+        <is>
+          <t>Agency test data</t>
+        </is>
+      </c>
+      <c r="F15" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to agency page
+2. Perform required actions
+3. Verify expected behavior</t>
+        </is>
+      </c>
+      <c r="G15" s="3" t="inlineStr">
+        <is>
+          <t>Agency functionality should work as expected</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="80" customHeight="1">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>TC_015</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>Verify that uploading PDF file shows validation message: 'Only accept jpg, png, jpeg, gif file'</t>
+        </is>
+      </c>
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>User is on the agency page</t>
+        </is>
+      </c>
+      <c r="E16" s="3" t="inlineStr">
+        <is>
+          <t>Agency test data</t>
+        </is>
+      </c>
+      <c r="F16" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to agency page
+2. Perform required actions
+3. Verify expected behavior</t>
+        </is>
+      </c>
+      <c r="G16" s="3" t="inlineStr">
+        <is>
+          <t>Agency functionality should work as expected</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="80" customHeight="1">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>TC_016</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>Verify that uploading file larger than 5MB shows validation message: 'File can't be larger than 5 MB'</t>
+        </is>
+      </c>
+      <c r="D17" s="3" t="inlineStr">
+        <is>
+          <t>User is on the agency page</t>
+        </is>
+      </c>
+      <c r="E17" s="3" t="inlineStr">
+        <is>
+          <t>Agency test data</t>
+        </is>
+      </c>
+      <c r="F17" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to agency page
+2. Perform required actions
+3. Verify expected behavior</t>
+        </is>
+      </c>
+      <c r="G17" s="3" t="inlineStr">
+        <is>
+          <t>Agency functionality should work as expected</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="80" customHeight="1">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>TC_017</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>Verify creating agency with image upload and verify it appears in list</t>
+        </is>
+      </c>
+      <c r="D18" s="3" t="inlineStr">
+        <is>
+          <t>User is on the agency page</t>
+        </is>
+      </c>
+      <c r="E18" s="3" t="inlineStr">
+        <is>
+          <t>Agency test data</t>
+        </is>
+      </c>
+      <c r="F18" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to agency page
+2. Perform required actions
+3. Verify expected behavior</t>
+        </is>
+      </c>
+      <c r="G18" s="3" t="inlineStr">
+        <is>
+          <t>Agency functionality should work as expected</t>
+        </is>
+      </c>
+      <c r="H18" s="3" t="inlineStr">
+        <is>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>

</xml_diff>